<commit_message>
Enter data for the following days, add the "Done" column
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Оля,\Оля МГУ\2к Inform\prog\MSU2023\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC329FFF-B059-4E14-9FED-9ED291B7F8E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -18,8 +24,31 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
+  <si>
+    <t xml:space="preserve">Д. з. </t>
+  </si>
+  <si>
+    <t>Информатика</t>
+  </si>
+  <si>
+    <t>Структурка</t>
+  </si>
+  <si>
+    <t>Эк. Геология</t>
+  </si>
+  <si>
+    <t>Д. з.</t>
+  </si>
+  <si>
+    <t>ТФКП</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -49,11 +78,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -330,13 +360,60 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="14.7109375" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1">
+        <v>44984</v>
+      </c>
+      <c r="B1" s="1">
+        <v>44985</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
write new home task
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Оля,\Оля МГУ\2к Inform\prog\MSU2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC329FFF-B059-4E14-9FED-9ED291B7F8E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB4834A4-FFD0-4114-A546-632537829CE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="11">
   <si>
     <t xml:space="preserve">Д. з. </t>
   </si>
@@ -39,10 +39,25 @@
     <t>Эк. Геология</t>
   </si>
   <si>
-    <t>Д. з.</t>
-  </si>
-  <si>
     <t>ТФКП</t>
+  </si>
+  <si>
+    <t>Степень выполнения</t>
+  </si>
+  <si>
+    <t>Выполнено</t>
+  </si>
+  <si>
+    <t>Яд. Физика</t>
+  </si>
+  <si>
+    <t>Не выполнено</t>
+  </si>
+  <si>
+    <t>В процессе</t>
+  </si>
+  <si>
+    <t>_</t>
   </si>
 </sst>
 </file>
@@ -361,56 +376,110 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" customWidth="1"/>
+    <col min="3" max="3" width="27.7109375" customWidth="1"/>
+    <col min="4" max="4" width="17.140625" customWidth="1"/>
+    <col min="5" max="5" width="13.140625" customWidth="1"/>
+    <col min="6" max="6" width="13.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
         <v>44984</v>
-      </c>
-      <c r="B1" s="1">
-        <v>44985</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>1</v>
       </c>
       <c r="B3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
         <v>2</v>
       </c>
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
         <v>3</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>44985</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
         <v>2</v>
+      </c>
+      <c r="C9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>44986</v>
+      </c>
+      <c r="B11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>